<commit_message>
descw-1282 get report populating properly
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
+++ b/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72405538-D5C9-DB4A-99AF-7109E3017FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9741B7-9D59-D24C-BD8F-5D337B7DCC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>{#t=d.report_totals}</t>
-  </si>
-  <si>
-    <t>{$t.sum}</t>
-  </si>
-  <si>
-    <t>{$r.sum}</t>
   </si>
   <si>
     <t>{$rows.resource_type}</t>
@@ -76,13 +70,22 @@
   </si>
   <si>
     <t>Amount Invoiced</t>
+  </si>
+  <si>
+    <t>{$t.total}</t>
+  </si>
+  <si>
+    <t>{$rows.total}</t>
+  </si>
+  <si>
+    <t>{$row.total}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,14 +108,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -122,7 +117,7 @@
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +136,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -230,7 +231,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
       <right/>
       <top style="medium">
         <color rgb="FFBFBFBF"/>
@@ -253,34 +256,34 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -290,6 +293,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD9D9D9"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -663,7 +667,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -677,52 +681,54 @@
     <row r="1" spans="1:3" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="19">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="6"/>
-    </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19">

</xml_diff>

<commit_message>
descw-1282 refactor template and model
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
+++ b/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9741B7-9D59-D24C-BD8F-5D337B7DCC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6FEC5D-82E9-2944-B2FD-CD41EB443AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -44,13 +44,7 @@
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
     <t>{#t=d.report_totals}</t>
-  </si>
-  <si>
-    <t>{$rows.resource_type}</t>
   </si>
   <si>
     <t>{$row.resource_type}</t>
@@ -75,17 +69,17 @@
     <t>{$t.total}</t>
   </si>
   <si>
-    <t>{$rows.total}</t>
-  </si>
-  <si>
     <t>{$row.total}</t>
+  </si>
+  <si>
+    <t>{$rows}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +89,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
@@ -108,16 +107,17 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,20 +130,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -151,139 +139,28 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,99 +541,113 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="83" customHeight="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="19">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="19">
-      <c r="A2" s="7" t="s">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="19">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="19">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="19">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="10" t="s">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="19">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="19">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="19">
+      <c r="A9"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="19">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="19">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="10" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" ht="19">
+      <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="12" t="s">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" ht="19">
+      <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="19">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="19">
-      <c r="A12" s="3" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="19">
+      <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="19">
-      <c r="A13" s="3" t="s">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="19">
+      <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B15" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
descw-1282 make report look nice(er)
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
+++ b/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6FEC5D-82E9-2944-B2FD-CD41EB443AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FF09EB-5D07-9B4A-A121-018B5A2C21C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>{#date=d.date}</t>
   </si>
   <si>
     <t>{#fy=d.fiscal_year}</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
   <si>
     <t>{#t=d.report_totals}</t>
@@ -79,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,8 +119,13 @@
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +138,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,11 +153,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -161,6 +186,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,13 +581,13 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="69.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="9" width="15.83203125" customWidth="1"/>
   </cols>
@@ -558,39 +595,41 @@
     <row r="1" spans="1:3" s="1" customFormat="1" ht="83" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="19">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="23" customHeight="1" thickBot="1">
+      <c r="A2" s="10" t="s">
         <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" ht="19">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="19">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="19">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -599,52 +638,49 @@
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="19">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="21">
+      <c r="A7" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="21">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="19">
-      <c r="A9"/>
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="21">
+      <c r="A9" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="19">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="21">
+      <c r="A10" s="11" t="s">
+        <v>1</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" ht="19">
-      <c r="A11" s="4" t="s">
-        <v>5</v>
+    <row r="11" spans="1:3" ht="21">
+      <c r="A11" s="11" t="s">
+        <v>0</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="19">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="19">
-      <c r="A13" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="19">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:3" ht="19">
-      <c r="A15" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="B15" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
descw-1282 optimize model operations
* also update formatting on Template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
+++ b/backend/reports/xlsx/Tab_5_rpt_CA_ConsultingServiceUtilization-FY-Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FF09EB-5D07-9B4A-A121-018B5A2C21C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23998453-5EFD-A54B-8FA8-A2461E422050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>{#t=d.report_totals}</t>
-  </si>
-  <si>
     <t>{$row.resource_type}</t>
   </si>
   <si>
@@ -69,13 +66,16 @@
     <t>Amount Invoiced</t>
   </si>
   <si>
-    <t>{$t.total}</t>
-  </si>
-  <si>
     <t>{$row.total}</t>
   </si>
   <si>
     <t>{$rows}</t>
+  </si>
+  <si>
+    <t>{#t=d.report_total}</t>
+  </si>
+  <si>
+    <t>{$t}</t>
   </si>
 </sst>
 </file>
@@ -178,19 +178,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -581,7 +581,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -595,31 +595,31 @@
     <row r="1" spans="1:3" s="1" customFormat="1" ht="83" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="23" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" ht="19">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="19">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -640,20 +640,20 @@
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="21">
       <c r="A7" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="21">
       <c r="A8" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="21">
       <c r="A9" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>

</xml_diff>